<commit_message>
Added more simple method for work with fields in class TO
</commit_message>
<xml_diff>
--- a/src/test/resources/rent_list.xlsx
+++ b/src/test/resources/rent_list.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="435" windowWidth="14040" windowHeight="4545"/>
+    <workbookView xWindow="90" yWindow="435" windowWidth="14040" windowHeight="4545" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Rent Data" sheetId="1" r:id="rId1"/>
+    <sheet name="test" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="335">
   <si>
     <t>aviso</t>
   </si>
@@ -731,19 +732,315 @@
   </si>
   <si>
     <t>http://odessa.od.slando.ua/obyavlenie/sdaetsya-uyutnyy-dom-6-st-lyustdorfskoy-dorogi-odessa-ID7AjEf.html</t>
+  </si>
+  <si>
+    <t>21-12-2013 / 13:49:52</t>
+  </si>
+  <si>
+    <t>1 комн. в центре на ул. Приморская(008)</t>
+  </si>
+  <si>
+    <t>Сегодня 13:51</t>
+  </si>
+  <si>
+    <t>http://odessa.od.slando.ua/obyavlenie/1-komn-v-tsentre-na-ul-primorskaya008-ID87HOw.html</t>
+  </si>
+  <si>
+    <t>, Суворовский, Посёлок Котовского</t>
+  </si>
+  <si>
+    <t>2-х квартира на Днепродороге парковая зона</t>
+  </si>
+  <si>
+    <t>3 100 грн.</t>
+  </si>
+  <si>
+    <t>Сегодня 13:49</t>
+  </si>
+  <si>
+    <t>http://odessa.od.slando.ua/obyavlenie/2-h-kvartira-na-dneprodoroge-parkovaya-zona-ID7PWSz.html</t>
+  </si>
+  <si>
+    <t>, Приморский, Ольгиевская / Княжеская</t>
+  </si>
+  <si>
+    <t>Сдам 1 комнатную квартиру</t>
+  </si>
+  <si>
+    <t>Сегодня 13:47</t>
+  </si>
+  <si>
+    <t>http://odessa.od.slando.ua/obyavlenie/sdam-1-komnatnuyu-kvartiru-ID7oScN.html</t>
+  </si>
+  <si>
+    <t>, Академика Филатова</t>
+  </si>
+  <si>
+    <t>сдам 2 квартиру Филатова/солнечное</t>
+  </si>
+  <si>
+    <t>Сегодня 13:46</t>
+  </si>
+  <si>
+    <t>http://odessa.od.slando.ua/obyavlenie/sdam-2-kvartiru-filatova-solnechnoe-ID5jafj.html</t>
+  </si>
+  <si>
+    <t>, Приморский, Тираспольская</t>
+  </si>
+  <si>
+    <t>сда 2х.к.кв тираспольская</t>
+  </si>
+  <si>
+    <t>4 000 грн.</t>
+  </si>
+  <si>
+    <t>http://odessa.od.slando.ua/obyavlenie/sda-2h-k-kv-tiraspolskaya-ID6Uglr.html</t>
+  </si>
+  <si>
+    <t>2х комн. кв. в центре Ришельевская (004)</t>
+  </si>
+  <si>
+    <t>6 500 грн.</t>
+  </si>
+  <si>
+    <t>Сегодня 13:44</t>
+  </si>
+  <si>
+    <t>http://odessa.od.slando.ua/obyavlenie/2h-komn-kv-v-tsentre-rishelevskaya-004-ID87Ab3.html</t>
+  </si>
+  <si>
+    <t>, Еврейская/Осипова</t>
+  </si>
+  <si>
+    <t>Сдам квартиру-студию в центре</t>
+  </si>
+  <si>
+    <t>http://odessa.od.slando.ua/obyavlenie/sdam-kvartiru-studiyu-v-tsentre-ID5AuP9.html</t>
+  </si>
+  <si>
+    <t>, Приморский, греческая</t>
+  </si>
+  <si>
+    <t>Сдам 2-Х ком.кв.центр</t>
+  </si>
+  <si>
+    <t>Сегодня 13:42</t>
+  </si>
+  <si>
+    <t>http://odessa.od.slando.ua/obyavlenie/sdam-2-h-kom-kv-tsentr-ID8b2IZ.html</t>
+  </si>
+  <si>
+    <t>, Киевский, Королёва/Костанди</t>
+  </si>
+  <si>
+    <t>Сдам квартиру кухня-студия+спальня на Королёва</t>
+  </si>
+  <si>
+    <t>http://odessa.od.slando.ua/obyavlenie/sdam-kvartiru-kuhnya-studiya-spalnya-na-koroleva-ID87IST.html</t>
+  </si>
+  <si>
+    <t>Сдам квартиру-студию на Раскидайловской</t>
+  </si>
+  <si>
+    <t>http://odessa.od.slando.ua/obyavlenie/sdam-kvartiru-studiyu-na-raskidaylovskoy-ID72zJX.html</t>
+  </si>
+  <si>
+    <t>, Приморский, Б Арнаутская</t>
+  </si>
+  <si>
+    <t>Сдам 2-Х ком.кв.</t>
+  </si>
+  <si>
+    <t>4 500 грн.</t>
+  </si>
+  <si>
+    <t>Сегодня 13:41</t>
+  </si>
+  <si>
+    <t>http://odessa.od.slando.ua/obyavlenie/sdam-2-h-kom-kv-ID7IFxd.html</t>
+  </si>
+  <si>
+    <t>, Приморский, среднефонтанская</t>
+  </si>
+  <si>
+    <t>сдам 1 квартиру Среднефонтанская</t>
+  </si>
+  <si>
+    <t>2 900 грн.</t>
+  </si>
+  <si>
+    <t>Сегодня 13:40</t>
+  </si>
+  <si>
+    <t>http://odessa.od.slando.ua/obyavlenie/sdam-1-kvartiru-srednefontanskaya-ID6Oez3.html</t>
+  </si>
+  <si>
+    <t>, Приморский, Троицкая/Александровский пр-т</t>
+  </si>
+  <si>
+    <t>Сдам 1-ную квартиру</t>
+  </si>
+  <si>
+    <t>6 104 грн.</t>
+  </si>
+  <si>
+    <t>Сегодня 13:39</t>
+  </si>
+  <si>
+    <t>http://odessa.od.slando.ua/obyavlenie/sdam-1-nuyu-kvartiru-ID8b3pW.html</t>
+  </si>
+  <si>
+    <t>, Малиновский, Варненская</t>
+  </si>
+  <si>
+    <t>Сдам 2-х комнатную квартиру на Черёмушках</t>
+  </si>
+  <si>
+    <t>Сегодня 13:36</t>
+  </si>
+  <si>
+    <t>http://odessa.od.slando.ua/obyavlenie/sdam-2-h-komnatnuyu-kvartiru-na-cheremushkah-ID87IKz.html</t>
+  </si>
+  <si>
+    <t>хорошая 1 комн недорого Бочарова</t>
+  </si>
+  <si>
+    <t>1 800 грн.</t>
+  </si>
+  <si>
+    <t>http://odessa.od.slando.ua/obyavlenie/horoshaya-1-komn-nedorogo-bocharova-ID8bswh.html</t>
+  </si>
+  <si>
+    <t>, Приморский, Старосеннная площадь</t>
+  </si>
+  <si>
+    <t>Выделенная коммуна на Старосеной площади</t>
+  </si>
+  <si>
+    <t>3 250 грн.</t>
+  </si>
+  <si>
+    <t>http://odessa.od.slando.ua/obyavlenie/vydelennaya-kommuna-na-starosenoy-ploschadi-ID87LC5.html</t>
+  </si>
+  <si>
+    <t>, Приморский, приморский</t>
+  </si>
+  <si>
+    <t>Cдам 1-ком.в центре</t>
+  </si>
+  <si>
+    <t>Сегодня 13:35</t>
+  </si>
+  <si>
+    <t>http://odessa.od.slando.ua/obyavlenie/cdam-1-kom-v-tsentre-ID6ZOQP.html</t>
+  </si>
+  <si>
+    <t>, Ильфа и петрова 8</t>
+  </si>
+  <si>
+    <t>Сдам 1 квартиру Ильфа и Петрова</t>
+  </si>
+  <si>
+    <t>Сегодня 13:34</t>
+  </si>
+  <si>
+    <t>http://odessa.od.slando.ua/obyavlenie/sdam-1-kvartiru-ilfa-i-petrova-ID59JXN.html</t>
+  </si>
+  <si>
+    <t>, Киевский, Люстдорфская дорога</t>
+  </si>
+  <si>
+    <t>Сдам 2-х комнатную на люстдорфской дороге</t>
+  </si>
+  <si>
+    <t>http://odessa.od.slando.ua/obyavlenie/sdam-2-h-komnatnuyu-na-lyustdorfskoy-doroge-ID7YkFx.html</t>
+  </si>
+  <si>
+    <t>, Приморский, Ул. Кузнечная</t>
+  </si>
+  <si>
+    <t>Сегодня 13:33</t>
+  </si>
+  <si>
+    <t>http://odessa.od.slando.ua/obyavlenie/sdam-1-komnatnuyu-kvartiru-ID7cn1r.html</t>
+  </si>
+  <si>
+    <t>, Приморский, большая арнаутская 57</t>
+  </si>
+  <si>
+    <t>сдам 2 квартиру Большая арнаутская</t>
+  </si>
+  <si>
+    <t>Сегодня 13:31</t>
+  </si>
+  <si>
+    <t>http://odessa.od.slando.ua/obyavlenie/sdam-2-kvartiru-bolshaya-arnautskaya-ID7oDLn.html</t>
+  </si>
+  <si>
+    <t>, Приморский, Кленовая</t>
+  </si>
+  <si>
+    <t>Сдам 2-х комнатную квартиру на Кленовой</t>
+  </si>
+  <si>
+    <t>5 697 грн.</t>
+  </si>
+  <si>
+    <t>http://odessa.od.slando.ua/obyavlenie/sdam-2-h-komnatnuyu-kvartiru-na-klenovoy-ID87IDb.html</t>
+  </si>
+  <si>
+    <t>, Рaзумовскя</t>
+  </si>
+  <si>
+    <t>Сдам 2х комн.квартиру,с рaздельными ходaми</t>
+  </si>
+  <si>
+    <t>Сегодня 13:29</t>
+  </si>
+  <si>
+    <t>http://odessa.od.slando.ua/obyavlenie/sdam-2h-komn-kvartiru-s-razdelnymi-hodami-ID4Yrbd.html</t>
+  </si>
+  <si>
+    <t>, Приморский, приморский р-н</t>
+  </si>
+  <si>
+    <t>Сдам 2-Х ком.квартиру,в центре города,</t>
+  </si>
+  <si>
+    <t>4 883 грн.</t>
+  </si>
+  <si>
+    <t>http://odessa.od.slando.ua/obyavlenie/sdam-2-h-kom-kvartiru-v-tsentre-goroda-ID8b32l.html</t>
+  </si>
+  <si>
+    <t>Срочно квартира Базарная|ЖК Капитан,2раздельные спальни,+кухня</t>
+  </si>
+  <si>
+    <t>Сегодня 13:28</t>
+  </si>
+  <si>
+    <t>http://odessa.od.slando.ua/obyavlenie/srochno-kvartira-bazarnaya-zhk-kapitan-2razdelnye-spalni-kuhnya-ID8849d.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -767,8 +1064,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1070,23 +1368,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="G1"/>
+  <dimension ref="A1:G110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A85" sqref="A84:XFD85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="43.28515625" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="71.42578125" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="31.28515625" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="26.0" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="49.85546875" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="2" max="2" width="43.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="71.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="26" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="49.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="25.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1109,7 +1407,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1132,7 +1430,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1155,7 +1453,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1178,7 +1476,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1201,7 +1499,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1224,7 +1522,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1247,7 +1545,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1270,7 +1568,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1293,7 +1591,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1316,7 +1614,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1339,7 +1637,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1362,7 +1660,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1385,7 +1683,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1408,7 +1706,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1431,7 +1729,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1454,7 +1752,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1477,7 +1775,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -1500,7 +1798,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1523,7 +1821,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1546,7 +1844,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -1569,7 +1867,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -1592,7 +1890,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -1615,7 +1913,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1638,7 +1936,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -1661,7 +1959,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -1684,7 +1982,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -1707,7 +2005,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -1730,7 +2028,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -1753,7 +2051,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -1776,7 +2074,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>134</v>
       </c>
@@ -1799,7 +2097,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>134</v>
       </c>
@@ -1822,7 +2120,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>134</v>
       </c>
@@ -1845,7 +2143,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>134</v>
       </c>
@@ -1868,7 +2166,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>134</v>
       </c>
@@ -1891,7 +2189,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>134</v>
       </c>
@@ -1914,7 +2212,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>134</v>
       </c>
@@ -1937,7 +2235,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>134</v>
       </c>
@@ -1960,7 +2258,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>134</v>
       </c>
@@ -1983,7 +2281,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>134</v>
       </c>
@@ -2006,7 +2304,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>134</v>
       </c>
@@ -2029,7 +2327,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>134</v>
       </c>
@@ -2052,7 +2350,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>134</v>
       </c>
@@ -2075,7 +2373,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>134</v>
       </c>
@@ -2098,7 +2396,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>134</v>
       </c>
@@ -2121,7 +2419,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>134</v>
       </c>
@@ -2144,7 +2442,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>134</v>
       </c>
@@ -2167,7 +2465,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>134</v>
       </c>
@@ -2190,7 +2488,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>134</v>
       </c>
@@ -2213,7 +2511,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>134</v>
       </c>
@@ -2236,7 +2534,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>134</v>
       </c>
@@ -2259,7 +2557,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>134</v>
       </c>
@@ -2282,7 +2580,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>134</v>
       </c>
@@ -2305,7 +2603,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>134</v>
       </c>
@@ -2328,7 +2626,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>134</v>
       </c>
@@ -2351,7 +2649,1285 @@
         <v>6</v>
       </c>
     </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56" t="s">
+        <v>85</v>
+      </c>
+      <c r="C56" t="s">
+        <v>86</v>
+      </c>
+      <c r="D56" t="s">
+        <v>87</v>
+      </c>
+      <c r="E56" t="s">
+        <v>239</v>
+      </c>
+      <c r="F56" t="s">
+        <v>89</v>
+      </c>
+      <c r="G56" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57" t="s">
+        <v>2</v>
+      </c>
+      <c r="D57" t="s">
+        <v>3</v>
+      </c>
+      <c r="E57" t="s">
+        <v>4</v>
+      </c>
+      <c r="F57" t="s">
+        <v>5</v>
+      </c>
+      <c r="G57" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" t="s">
+        <v>8</v>
+      </c>
+      <c r="D58" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" t="s">
+        <v>4</v>
+      </c>
+      <c r="F58" t="s">
+        <v>10</v>
+      </c>
+      <c r="G58" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" t="s">
+        <v>11</v>
+      </c>
+      <c r="C59" t="s">
+        <v>12</v>
+      </c>
+      <c r="D59" t="s">
+        <v>13</v>
+      </c>
+      <c r="E59" t="s">
+        <v>14</v>
+      </c>
+      <c r="F59" t="s">
+        <v>15</v>
+      </c>
+      <c r="G59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" t="s">
+        <v>16</v>
+      </c>
+      <c r="C60" t="s">
+        <v>17</v>
+      </c>
+      <c r="D60" t="s">
+        <v>18</v>
+      </c>
+      <c r="E60" t="s">
+        <v>19</v>
+      </c>
+      <c r="F60" t="s">
+        <v>20</v>
+      </c>
+      <c r="G60" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" t="s">
+        <v>21</v>
+      </c>
+      <c r="C61" t="s">
+        <v>22</v>
+      </c>
+      <c r="D61" t="s">
+        <v>23</v>
+      </c>
+      <c r="E61" t="s">
+        <v>24</v>
+      </c>
+      <c r="F61" t="s">
+        <v>25</v>
+      </c>
+      <c r="G61" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>0</v>
+      </c>
+      <c r="B62" t="s">
+        <v>26</v>
+      </c>
+      <c r="C62" t="s">
+        <v>27</v>
+      </c>
+      <c r="D62" t="s">
+        <v>28</v>
+      </c>
+      <c r="E62" t="s">
+        <v>29</v>
+      </c>
+      <c r="F62" t="s">
+        <v>30</v>
+      </c>
+      <c r="G62" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>0</v>
+      </c>
+      <c r="B63" t="s">
+        <v>31</v>
+      </c>
+      <c r="C63" t="s">
+        <v>32</v>
+      </c>
+      <c r="D63" t="s">
+        <v>33</v>
+      </c>
+      <c r="E63" t="s">
+        <v>34</v>
+      </c>
+      <c r="F63" t="s">
+        <v>35</v>
+      </c>
+      <c r="G63" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>0</v>
+      </c>
+      <c r="B64" t="s">
+        <v>36</v>
+      </c>
+      <c r="C64" t="s">
+        <v>37</v>
+      </c>
+      <c r="D64" t="s">
+        <v>38</v>
+      </c>
+      <c r="E64" t="s">
+        <v>34</v>
+      </c>
+      <c r="F64" t="s">
+        <v>39</v>
+      </c>
+      <c r="G64" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>0</v>
+      </c>
+      <c r="B65" t="s">
+        <v>40</v>
+      </c>
+      <c r="C65" t="s">
+        <v>41</v>
+      </c>
+      <c r="D65" t="s">
+        <v>42</v>
+      </c>
+      <c r="E65" t="s">
+        <v>34</v>
+      </c>
+      <c r="F65" t="s">
+        <v>43</v>
+      </c>
+      <c r="G65" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>0</v>
+      </c>
+      <c r="B66" t="s">
+        <v>44</v>
+      </c>
+      <c r="C66" t="s">
+        <v>45</v>
+      </c>
+      <c r="D66" t="s">
+        <v>23</v>
+      </c>
+      <c r="E66" t="s">
+        <v>34</v>
+      </c>
+      <c r="F66" t="s">
+        <v>46</v>
+      </c>
+      <c r="G66" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>0</v>
+      </c>
+      <c r="B67" t="s">
+        <v>47</v>
+      </c>
+      <c r="C67" t="s">
+        <v>48</v>
+      </c>
+      <c r="D67" t="s">
+        <v>49</v>
+      </c>
+      <c r="E67" t="s">
+        <v>34</v>
+      </c>
+      <c r="F67" t="s">
+        <v>50</v>
+      </c>
+      <c r="G67" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>0</v>
+      </c>
+      <c r="B68" t="s">
+        <v>51</v>
+      </c>
+      <c r="C68" t="s">
+        <v>52</v>
+      </c>
+      <c r="D68" t="s">
+        <v>53</v>
+      </c>
+      <c r="E68" t="s">
+        <v>34</v>
+      </c>
+      <c r="F68" t="s">
+        <v>54</v>
+      </c>
+      <c r="G68" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>0</v>
+      </c>
+      <c r="B69" t="s">
+        <v>55</v>
+      </c>
+      <c r="C69" t="s">
+        <v>56</v>
+      </c>
+      <c r="D69" t="s">
+        <v>57</v>
+      </c>
+      <c r="E69" t="s">
+        <v>34</v>
+      </c>
+      <c r="F69" t="s">
+        <v>58</v>
+      </c>
+      <c r="G69" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>0</v>
+      </c>
+      <c r="B70" t="s">
+        <v>59</v>
+      </c>
+      <c r="C70" t="s">
+        <v>60</v>
+      </c>
+      <c r="D70" t="s">
+        <v>53</v>
+      </c>
+      <c r="E70" t="s">
+        <v>34</v>
+      </c>
+      <c r="F70" t="s">
+        <v>61</v>
+      </c>
+      <c r="G70" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>0</v>
+      </c>
+      <c r="B71" t="s">
+        <v>62</v>
+      </c>
+      <c r="C71" t="s">
+        <v>63</v>
+      </c>
+      <c r="D71" t="s">
+        <v>64</v>
+      </c>
+      <c r="E71" t="s">
+        <v>34</v>
+      </c>
+      <c r="F71" t="s">
+        <v>65</v>
+      </c>
+      <c r="G71" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>0</v>
+      </c>
+      <c r="B72" t="s">
+        <v>66</v>
+      </c>
+      <c r="C72" t="s">
+        <v>67</v>
+      </c>
+      <c r="D72" t="s">
+        <v>68</v>
+      </c>
+      <c r="E72" t="s">
+        <v>34</v>
+      </c>
+      <c r="F72" t="s">
+        <v>69</v>
+      </c>
+      <c r="G72" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>0</v>
+      </c>
+      <c r="B73" t="s">
+        <v>70</v>
+      </c>
+      <c r="C73" t="s">
+        <v>71</v>
+      </c>
+      <c r="D73" t="s">
+        <v>72</v>
+      </c>
+      <c r="E73" t="s">
+        <v>73</v>
+      </c>
+      <c r="F73" t="s">
+        <v>74</v>
+      </c>
+      <c r="G73" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>0</v>
+      </c>
+      <c r="B74" t="s">
+        <v>75</v>
+      </c>
+      <c r="C74" t="s">
+        <v>76</v>
+      </c>
+      <c r="D74" t="s">
+        <v>77</v>
+      </c>
+      <c r="E74" t="s">
+        <v>78</v>
+      </c>
+      <c r="F74" t="s">
+        <v>79</v>
+      </c>
+      <c r="G74" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>0</v>
+      </c>
+      <c r="B75" t="s">
+        <v>80</v>
+      </c>
+      <c r="C75" t="s">
+        <v>81</v>
+      </c>
+      <c r="D75" t="s">
+        <v>82</v>
+      </c>
+      <c r="E75" t="s">
+        <v>83</v>
+      </c>
+      <c r="F75" t="s">
+        <v>84</v>
+      </c>
+      <c r="G75" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>0</v>
+      </c>
+      <c r="B76" t="s">
+        <v>90</v>
+      </c>
+      <c r="C76" t="s">
+        <v>91</v>
+      </c>
+      <c r="D76" t="s">
+        <v>92</v>
+      </c>
+      <c r="E76" t="s">
+        <v>93</v>
+      </c>
+      <c r="F76" t="s">
+        <v>94</v>
+      </c>
+      <c r="G76" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>0</v>
+      </c>
+      <c r="B77" t="s">
+        <v>95</v>
+      </c>
+      <c r="C77" t="s">
+        <v>96</v>
+      </c>
+      <c r="D77" t="s">
+        <v>97</v>
+      </c>
+      <c r="E77" t="s">
+        <v>98</v>
+      </c>
+      <c r="F77" t="s">
+        <v>99</v>
+      </c>
+      <c r="G77" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>0</v>
+      </c>
+      <c r="B78" t="s">
+        <v>100</v>
+      </c>
+      <c r="C78" t="s">
+        <v>101</v>
+      </c>
+      <c r="D78" t="s">
+        <v>102</v>
+      </c>
+      <c r="E78" t="s">
+        <v>103</v>
+      </c>
+      <c r="F78" t="s">
+        <v>104</v>
+      </c>
+      <c r="G78" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>0</v>
+      </c>
+      <c r="B79" t="s">
+        <v>105</v>
+      </c>
+      <c r="C79" t="s">
+        <v>106</v>
+      </c>
+      <c r="D79" t="s">
+        <v>107</v>
+      </c>
+      <c r="E79" t="s">
+        <v>108</v>
+      </c>
+      <c r="F79" t="s">
+        <v>109</v>
+      </c>
+      <c r="G79" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>0</v>
+      </c>
+      <c r="B80" t="s">
+        <v>110</v>
+      </c>
+      <c r="C80" t="s">
+        <v>111</v>
+      </c>
+      <c r="D80" t="s">
+        <v>112</v>
+      </c>
+      <c r="E80" t="s">
+        <v>108</v>
+      </c>
+      <c r="F80" t="s">
+        <v>113</v>
+      </c>
+      <c r="G80" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>0</v>
+      </c>
+      <c r="B81" t="s">
+        <v>114</v>
+      </c>
+      <c r="C81" t="s">
+        <v>115</v>
+      </c>
+      <c r="D81" t="s">
+        <v>97</v>
+      </c>
+      <c r="E81" t="s">
+        <v>108</v>
+      </c>
+      <c r="F81" t="s">
+        <v>116</v>
+      </c>
+      <c r="G81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>0</v>
+      </c>
+      <c r="B82" t="s">
+        <v>117</v>
+      </c>
+      <c r="C82" t="s">
+        <v>118</v>
+      </c>
+      <c r="D82" t="s">
+        <v>119</v>
+      </c>
+      <c r="E82" t="s">
+        <v>120</v>
+      </c>
+      <c r="F82" t="s">
+        <v>121</v>
+      </c>
+      <c r="G82" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>0</v>
+      </c>
+      <c r="B83" t="s">
+        <v>122</v>
+      </c>
+      <c r="C83" t="s">
+        <v>123</v>
+      </c>
+      <c r="D83" t="s">
+        <v>124</v>
+      </c>
+      <c r="E83" t="s">
+        <v>120</v>
+      </c>
+      <c r="F83" t="s">
+        <v>125</v>
+      </c>
+      <c r="G83" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>134</v>
+      </c>
+      <c r="B86" t="s">
+        <v>201</v>
+      </c>
+      <c r="C86" t="s">
+        <v>240</v>
+      </c>
+      <c r="D86" t="s">
+        <v>142</v>
+      </c>
+      <c r="E86" t="s">
+        <v>241</v>
+      </c>
+      <c r="F86" t="s">
+        <v>242</v>
+      </c>
+      <c r="G86" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>134</v>
+      </c>
+      <c r="B87" t="s">
+        <v>243</v>
+      </c>
+      <c r="C87" t="s">
+        <v>244</v>
+      </c>
+      <c r="D87" t="s">
+        <v>245</v>
+      </c>
+      <c r="E87" t="s">
+        <v>246</v>
+      </c>
+      <c r="F87" t="s">
+        <v>247</v>
+      </c>
+      <c r="G87" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>134</v>
+      </c>
+      <c r="B88" t="s">
+        <v>248</v>
+      </c>
+      <c r="C88" t="s">
+        <v>249</v>
+      </c>
+      <c r="D88" t="s">
+        <v>183</v>
+      </c>
+      <c r="E88" t="s">
+        <v>250</v>
+      </c>
+      <c r="F88" t="s">
+        <v>251</v>
+      </c>
+      <c r="G88" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>134</v>
+      </c>
+      <c r="B89" t="s">
+        <v>252</v>
+      </c>
+      <c r="C89" t="s">
+        <v>253</v>
+      </c>
+      <c r="D89" t="s">
+        <v>152</v>
+      </c>
+      <c r="E89" t="s">
+        <v>254</v>
+      </c>
+      <c r="F89" t="s">
+        <v>255</v>
+      </c>
+      <c r="G89" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>134</v>
+      </c>
+      <c r="B90" t="s">
+        <v>256</v>
+      </c>
+      <c r="C90" t="s">
+        <v>257</v>
+      </c>
+      <c r="D90" t="s">
+        <v>258</v>
+      </c>
+      <c r="E90" t="s">
+        <v>254</v>
+      </c>
+      <c r="F90" t="s">
+        <v>259</v>
+      </c>
+      <c r="G90" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>134</v>
+      </c>
+      <c r="B91" t="s">
+        <v>201</v>
+      </c>
+      <c r="C91" t="s">
+        <v>260</v>
+      </c>
+      <c r="D91" t="s">
+        <v>261</v>
+      </c>
+      <c r="E91" t="s">
+        <v>262</v>
+      </c>
+      <c r="F91" t="s">
+        <v>263</v>
+      </c>
+      <c r="G91" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>134</v>
+      </c>
+      <c r="B92" t="s">
+        <v>264</v>
+      </c>
+      <c r="C92" t="s">
+        <v>265</v>
+      </c>
+      <c r="D92" t="s">
+        <v>147</v>
+      </c>
+      <c r="E92" t="s">
+        <v>262</v>
+      </c>
+      <c r="F92" t="s">
+        <v>266</v>
+      </c>
+      <c r="G92" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>134</v>
+      </c>
+      <c r="B93" t="s">
+        <v>267</v>
+      </c>
+      <c r="C93" t="s">
+        <v>268</v>
+      </c>
+      <c r="D93" t="s">
+        <v>229</v>
+      </c>
+      <c r="E93" t="s">
+        <v>269</v>
+      </c>
+      <c r="F93" t="s">
+        <v>270</v>
+      </c>
+      <c r="G93" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>134</v>
+      </c>
+      <c r="B94" t="s">
+        <v>271</v>
+      </c>
+      <c r="C94" t="s">
+        <v>272</v>
+      </c>
+      <c r="D94" t="s">
+        <v>157</v>
+      </c>
+      <c r="E94" t="s">
+        <v>269</v>
+      </c>
+      <c r="F94" t="s">
+        <v>273</v>
+      </c>
+      <c r="G94" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>134</v>
+      </c>
+      <c r="B95" t="s">
+        <v>201</v>
+      </c>
+      <c r="C95" t="s">
+        <v>274</v>
+      </c>
+      <c r="D95" t="s">
+        <v>183</v>
+      </c>
+      <c r="E95" t="s">
+        <v>269</v>
+      </c>
+      <c r="F95" t="s">
+        <v>275</v>
+      </c>
+      <c r="G95" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>134</v>
+      </c>
+      <c r="B96" t="s">
+        <v>276</v>
+      </c>
+      <c r="C96" t="s">
+        <v>277</v>
+      </c>
+      <c r="D96" t="s">
+        <v>278</v>
+      </c>
+      <c r="E96" t="s">
+        <v>279</v>
+      </c>
+      <c r="F96" t="s">
+        <v>280</v>
+      </c>
+      <c r="G96" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>134</v>
+      </c>
+      <c r="B97" t="s">
+        <v>281</v>
+      </c>
+      <c r="C97" t="s">
+        <v>282</v>
+      </c>
+      <c r="D97" t="s">
+        <v>283</v>
+      </c>
+      <c r="E97" t="s">
+        <v>284</v>
+      </c>
+      <c r="F97" t="s">
+        <v>285</v>
+      </c>
+      <c r="G97" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>134</v>
+      </c>
+      <c r="B98" t="s">
+        <v>286</v>
+      </c>
+      <c r="C98" t="s">
+        <v>287</v>
+      </c>
+      <c r="D98" t="s">
+        <v>288</v>
+      </c>
+      <c r="E98" t="s">
+        <v>289</v>
+      </c>
+      <c r="F98" t="s">
+        <v>290</v>
+      </c>
+      <c r="G98" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>134</v>
+      </c>
+      <c r="B99" t="s">
+        <v>291</v>
+      </c>
+      <c r="C99" t="s">
+        <v>292</v>
+      </c>
+      <c r="D99" t="s">
+        <v>142</v>
+      </c>
+      <c r="E99" t="s">
+        <v>293</v>
+      </c>
+      <c r="F99" t="s">
+        <v>294</v>
+      </c>
+      <c r="G99" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>134</v>
+      </c>
+      <c r="B100" t="s">
+        <v>243</v>
+      </c>
+      <c r="C100" t="s">
+        <v>295</v>
+      </c>
+      <c r="D100" t="s">
+        <v>296</v>
+      </c>
+      <c r="E100" t="s">
+        <v>293</v>
+      </c>
+      <c r="F100" t="s">
+        <v>297</v>
+      </c>
+      <c r="G100" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>134</v>
+      </c>
+      <c r="B101" t="s">
+        <v>298</v>
+      </c>
+      <c r="C101" t="s">
+        <v>299</v>
+      </c>
+      <c r="D101" t="s">
+        <v>300</v>
+      </c>
+      <c r="E101" t="s">
+        <v>293</v>
+      </c>
+      <c r="F101" t="s">
+        <v>301</v>
+      </c>
+      <c r="G101" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>134</v>
+      </c>
+      <c r="B102" t="s">
+        <v>302</v>
+      </c>
+      <c r="C102" t="s">
+        <v>303</v>
+      </c>
+      <c r="D102" t="s">
+        <v>183</v>
+      </c>
+      <c r="E102" t="s">
+        <v>304</v>
+      </c>
+      <c r="F102" t="s">
+        <v>305</v>
+      </c>
+      <c r="G102" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>134</v>
+      </c>
+      <c r="B103" t="s">
+        <v>306</v>
+      </c>
+      <c r="C103" t="s">
+        <v>307</v>
+      </c>
+      <c r="D103" t="s">
+        <v>179</v>
+      </c>
+      <c r="E103" t="s">
+        <v>308</v>
+      </c>
+      <c r="F103" t="s">
+        <v>309</v>
+      </c>
+      <c r="G103" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>134</v>
+      </c>
+      <c r="B104" t="s">
+        <v>310</v>
+      </c>
+      <c r="C104" t="s">
+        <v>311</v>
+      </c>
+      <c r="D104" t="s">
+        <v>157</v>
+      </c>
+      <c r="E104" t="s">
+        <v>308</v>
+      </c>
+      <c r="F104" t="s">
+        <v>312</v>
+      </c>
+      <c r="G104" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>134</v>
+      </c>
+      <c r="B105" t="s">
+        <v>313</v>
+      </c>
+      <c r="C105" t="s">
+        <v>249</v>
+      </c>
+      <c r="D105" t="s">
+        <v>147</v>
+      </c>
+      <c r="E105" t="s">
+        <v>314</v>
+      </c>
+      <c r="F105" t="s">
+        <v>315</v>
+      </c>
+      <c r="G105" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>134</v>
+      </c>
+      <c r="B106" t="s">
+        <v>316</v>
+      </c>
+      <c r="C106" t="s">
+        <v>317</v>
+      </c>
+      <c r="D106" t="s">
+        <v>147</v>
+      </c>
+      <c r="E106" t="s">
+        <v>318</v>
+      </c>
+      <c r="F106" t="s">
+        <v>319</v>
+      </c>
+      <c r="G106" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>134</v>
+      </c>
+      <c r="B107" t="s">
+        <v>320</v>
+      </c>
+      <c r="C107" t="s">
+        <v>321</v>
+      </c>
+      <c r="D107" t="s">
+        <v>322</v>
+      </c>
+      <c r="E107" t="s">
+        <v>318</v>
+      </c>
+      <c r="F107" t="s">
+        <v>323</v>
+      </c>
+      <c r="G107" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>134</v>
+      </c>
+      <c r="B108" t="s">
+        <v>324</v>
+      </c>
+      <c r="C108" t="s">
+        <v>325</v>
+      </c>
+      <c r="D108" t="s">
+        <v>162</v>
+      </c>
+      <c r="E108" t="s">
+        <v>326</v>
+      </c>
+      <c r="F108" t="s">
+        <v>327</v>
+      </c>
+      <c r="G108" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>134</v>
+      </c>
+      <c r="B109" t="s">
+        <v>328</v>
+      </c>
+      <c r="C109" t="s">
+        <v>329</v>
+      </c>
+      <c r="D109" t="s">
+        <v>330</v>
+      </c>
+      <c r="E109" t="s">
+        <v>326</v>
+      </c>
+      <c r="F109" t="s">
+        <v>331</v>
+      </c>
+      <c r="G109" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>134</v>
+      </c>
+      <c r="B110" t="s">
+        <v>186</v>
+      </c>
+      <c r="C110" t="s">
+        <v>332</v>
+      </c>
+      <c r="D110" t="s">
+        <v>322</v>
+      </c>
+      <c r="E110" t="s">
+        <v>333</v>
+      </c>
+      <c r="F110" t="s">
+        <v>334</v>
+      </c>
+      <c r="G110" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add some changes to pom.xml
</commit_message>
<xml_diff>
--- a/src/test/resources/rent_list.xlsx
+++ b/src/test/resources/rent_list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1316" uniqueCount="536">
   <si>
     <t>aviso</t>
   </si>
@@ -6050,6 +6050,282 @@
         <v>418</v>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>335</v>
+      </c>
+      <c r="B39" t="s">
+        <v>336</v>
+      </c>
+      <c r="C39" t="s">
+        <v>337</v>
+      </c>
+      <c r="D39" t="s">
+        <v>338</v>
+      </c>
+      <c r="E39" t="s">
+        <v>339</v>
+      </c>
+      <c r="F39" t="s">
+        <v>340</v>
+      </c>
+      <c r="G39" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>342</v>
+      </c>
+      <c r="B40" t="s">
+        <v>343</v>
+      </c>
+      <c r="C40" t="s">
+        <v>344</v>
+      </c>
+      <c r="D40" t="s">
+        <v>345</v>
+      </c>
+      <c r="E40" t="s">
+        <v>346</v>
+      </c>
+      <c r="F40" t="s">
+        <v>347</v>
+      </c>
+      <c r="G40" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>349</v>
+      </c>
+      <c r="B41" t="s">
+        <v>350</v>
+      </c>
+      <c r="C41" t="s">
+        <v>351</v>
+      </c>
+      <c r="D41" t="s">
+        <v>352</v>
+      </c>
+      <c r="E41" t="s">
+        <v>353</v>
+      </c>
+      <c r="F41" t="s">
+        <v>354</v>
+      </c>
+      <c r="G41" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>356</v>
+      </c>
+      <c r="B42" t="s">
+        <v>357</v>
+      </c>
+      <c r="C42" t="s">
+        <v>358</v>
+      </c>
+      <c r="D42" t="s">
+        <v>359</v>
+      </c>
+      <c r="E42" t="s">
+        <v>360</v>
+      </c>
+      <c r="F42" t="s">
+        <v>361</v>
+      </c>
+      <c r="G42" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>363</v>
+      </c>
+      <c r="B43" t="s">
+        <v>364</v>
+      </c>
+      <c r="C43" t="s">
+        <v>365</v>
+      </c>
+      <c r="D43" t="s">
+        <v>366</v>
+      </c>
+      <c r="E43" t="s">
+        <v>367</v>
+      </c>
+      <c r="F43" t="s">
+        <v>368</v>
+      </c>
+      <c r="G43" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>370</v>
+      </c>
+      <c r="B44" t="s">
+        <v>371</v>
+      </c>
+      <c r="C44" t="s">
+        <v>372</v>
+      </c>
+      <c r="D44" t="s">
+        <v>373</v>
+      </c>
+      <c r="E44" t="s">
+        <v>374</v>
+      </c>
+      <c r="F44" t="s">
+        <v>375</v>
+      </c>
+      <c r="G44" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>377</v>
+      </c>
+      <c r="B45" t="s">
+        <v>378</v>
+      </c>
+      <c r="C45" t="s">
+        <v>379</v>
+      </c>
+      <c r="D45" t="s">
+        <v>380</v>
+      </c>
+      <c r="E45" t="s">
+        <v>381</v>
+      </c>
+      <c r="F45" t="s">
+        <v>382</v>
+      </c>
+      <c r="G45" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>384</v>
+      </c>
+      <c r="B46" t="s">
+        <v>385</v>
+      </c>
+      <c r="C46" t="s">
+        <v>386</v>
+      </c>
+      <c r="D46" t="s">
+        <v>387</v>
+      </c>
+      <c r="E46" t="s">
+        <v>388</v>
+      </c>
+      <c r="F46" t="s">
+        <v>389</v>
+      </c>
+      <c r="G46" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>391</v>
+      </c>
+      <c r="B47" t="s">
+        <v>392</v>
+      </c>
+      <c r="C47" t="s">
+        <v>393</v>
+      </c>
+      <c r="D47" t="s">
+        <v>394</v>
+      </c>
+      <c r="E47" t="s">
+        <v>395</v>
+      </c>
+      <c r="F47" t="s">
+        <v>396</v>
+      </c>
+      <c r="G47" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>398</v>
+      </c>
+      <c r="B48" t="s">
+        <v>399</v>
+      </c>
+      <c r="C48" t="s">
+        <v>400</v>
+      </c>
+      <c r="D48" t="s">
+        <v>401</v>
+      </c>
+      <c r="E48" t="s">
+        <v>402</v>
+      </c>
+      <c r="F48" t="s">
+        <v>403</v>
+      </c>
+      <c r="G48" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>405</v>
+      </c>
+      <c r="B49" t="s">
+        <v>406</v>
+      </c>
+      <c r="C49" t="s">
+        <v>407</v>
+      </c>
+      <c r="D49" t="s">
+        <v>408</v>
+      </c>
+      <c r="E49" t="s">
+        <v>409</v>
+      </c>
+      <c r="F49" t="s">
+        <v>410</v>
+      </c>
+      <c r="G49" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>412</v>
+      </c>
+      <c r="B50" t="s">
+        <v>413</v>
+      </c>
+      <c r="C50" t="s">
+        <v>414</v>
+      </c>
+      <c r="D50" t="s">
+        <v>415</v>
+      </c>
+      <c r="E50" t="s">
+        <v>416</v>
+      </c>
+      <c r="F50" t="s">
+        <v>417</v>
+      </c>
+      <c r="G50" t="s">
+        <v>418</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>